<commit_message>
Title and FC issue
</commit_message>
<xml_diff>
--- a/club_names.xlsx
+++ b/club_names.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcuskarberg/Desktop/Competitor_price/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcuskarberg/Desktop/Football-Travel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AD4433-F859-5440-9444-7A9D982C338B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CED7DA-3578-9749-9CDD-9132063CB43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" activeTab="2" xr2:uid="{11594A43-A07C-9749-950F-F6643440C8D3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Arsenal</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>West Ham United</t>
-  </si>
-  <si>
-    <t>Teams in column A will be read</t>
-  </si>
-  <si>
-    <t>List of teams</t>
   </si>
   <si>
     <t>Lille</t>
@@ -552,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E59EE5-AAB7-EA4D-80FE-08D6137F1C18}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,100 +561,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -671,10 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{850AD82F-0095-EF4B-99B1-156ACADF9153}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:A20"/>
+      <selection sqref="A1:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -685,86 +672,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -774,17 +759,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -794,10 +774,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F6873-B513-5842-A138-E6EA9CAEFFD2}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,41 +788,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Olka, FRG, FT, app. Looking good
</commit_message>
<xml_diff>
--- a/club_names.xlsx
+++ b/club_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcuskarberg/Desktop/Football-Travel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CED7DA-3578-9749-9CDD-9132063CB43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D68FAF4-8D31-3248-985B-D1165013085F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" activeTab="2" xr2:uid="{11594A43-A07C-9749-950F-F6643440C8D3}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15720" xr2:uid="{11594A43-A07C-9749-950F-F6643440C8D3}"/>
   </bookViews>
   <sheets>
     <sheet name="EN" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Arsenal</t>
   </si>
@@ -161,12 +161,6 @@
   </si>
   <si>
     <t>Osasuna</t>
-  </si>
-  <si>
-    <t>Millwall</t>
-  </si>
-  <si>
-    <t>QPR</t>
   </si>
 </sst>
 </file>
@@ -546,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20E59EE5-AAB7-EA4D-80FE-08D6137F1C18}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,31 +617,21 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
@@ -776,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36F6873-B513-5842-A138-E6EA9CAEFFD2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>